<commit_message>
fix: correct seed file
</commit_message>
<xml_diff>
--- a/db/seeds/iching_data_ten_excel.xlsx
+++ b/db/seeds/iching_data_ten_excel.xlsx
@@ -37,8 +37,7 @@
     <t>image_sum</t>
   </si>
   <si>
-    <t xml:space="preserve">乾 (qián) / The Creative
-</t>
+    <t>乾 (qián) / The Creative</t>
   </si>
   <si>
     <t xml:space="preserve">In the dance of the cosmos, you stand at a moment rich with potential, where the energy of creation pulses strongly. Imagine dragons, majestic and auspicious, charting your path. Their presence heralds a period ripe for bold actions and new beginnings, a canvas awaiting the brush of your intentions.
@@ -149,8 +148,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">坤 (kūn) / The Receptive
-</t>
+    <t>坤 (kūn) / The Receptive</t>
   </si>
   <si>
     <t xml:space="preserve">In the silent stillness, you find yourself embraced by the essence of the receptive Earth, a realm where nurturing and patience reign supreme. This is a time to embody yin, the passive, yielding principle, suggesting a period of waiting, being open to the influences around you.
@@ -253,8 +251,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">屯 (zhūn) / Difficulty at the Beginning
-</t>
+    <t>屯 (zhūn) / Difficulty at the Beginning</t>
   </si>
   <si>
     <t xml:space="preserve">As you journey through life's tapestry, you find yourself amidst a phase of sprouting, where beginnings are budding, yet their outcomes are uncertain. It is like the early days of spring, where seeds are just starting to break through the soil, full of potential but not yet fully formed.
@@ -316,8 +313,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">蒙 (méng) / Youthful Folly
-</t>
+    <t>蒙 (méng) / Youthful Folly</t>
   </si>
   <si>
     <t xml:space="preserve">In the unfolding journey of your life, you find yourself in a phase akin to the student, eager to learn and grow. This period is marked by the pursuit of knowledge and understanding, a time to seek wisdom and gain insight.
@@ -386,8 +382,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">需 (xū) / Waiting
-</t>
+    <t>需 (xū) / Waiting</t>
   </si>
   <si>
     <t xml:space="preserve">As you navigate through the currents of life, you find yourself in a phase of waiting, akin to the calm before the rain. This period is marked by anticipation and preparation, a time to cultivate patience and trust in the natural flow of events.
@@ -450,8 +445,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">訟 (sòng) / Conflict
-</t>
+    <t>訟 (sòng) / Conflict</t>
   </si>
   <si>
     <t xml:space="preserve">As you journey through the intricate tapestry of life, you find yourself in a phase marked by a need for caution and discernment. This period is akin to reaching a great river, formidable and challenging to cross. It represents a time of potential conflict or misunderstanding, urging you to navigate carefully.
@@ -516,8 +510,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">師 (shī) / The Army
-</t>
+    <t>師 (shī) / The Army</t>
   </si>
   <si>
     <t xml:space="preserve">As you journey through life's rich landscape, you find yourself in a time reminiscent of an army preparing for a unified effort. This phase symbolizes organization, discipline, and collective action, highlighting the importance of cooperation and leadership.
@@ -584,8 +577,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">比 (bǐ) / Holding Together
-</t>
+    <t>比 (bǐ) / Holding Together</t>
   </si>
   <si>
     <t xml:space="preserve">In this chapter of your life's journey, you find yourself in a time reminiscent of gathering water, a symbol of seeking unity and connection. This phase is about building alliances, fostering community, and creating bonds based on shared values and mutual support.
@@ -663,8 +655,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">小畜 (xiǎo xù) / The Taming Power of the Small
-</t>
+    <t>小畜 (xiǎo xù) / The Taming Power of the Small</t>
   </si>
   <si>
     <t xml:space="preserve">In your life's journey, you find yourself in a phase akin to a gentle wind, slowly but steadily influencing its surroundings. This period is about subtle progress and small developments, emphasizing the power of patience and gradual influence.
@@ -725,7 +716,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">履 (lǚ) / Treading </t>
+    <t>履 (lǚ) / Treading</t>
   </si>
   <si>
     <t xml:space="preserve">In this phase of your life's journey, you find yourself on a path akin to treading carefully, like walking on the back of a tiger. This period speaks to the importance of cautious action and awareness of the consequences of your decisions.
@@ -1276,7 +1267,7 @@
     <col min="7" max="7" style="8" width="59.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1299,7 +1290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="1367.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="1274.25" customFormat="1" s="1">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>

</xml_diff>